<commit_message>
update for next release.
</commit_message>
<xml_diff>
--- a/docs/WorkingStatus.xlsx
+++ b/docs/WorkingStatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kitoh\Documents\AliceConv\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kitoh\source\aliceconv\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2751BCBF-85F4-494D-A9EC-700B398902E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D87967-9BAE-48C0-8A00-E041049E2433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1335" windowWidth="21330" windowHeight="15900" activeTab="1" xr2:uid="{FF061521-1F21-4413-9E31-090A18910087}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{FF061521-1F21-4413-9E31-090A18910087}"/>
   </bookViews>
   <sheets>
     <sheet name="CG" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="101">
   <si>
     <t>リトルプリンセス</t>
   </si>
@@ -416,6 +416,10 @@
   </si>
   <si>
     <t>〇 (PSG)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〇 (PC88MML)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1619,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8125B7-A0B0-4490-A0D0-BEF54767802B}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1730,6 +1734,9 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
@@ -1746,6 +1753,9 @@
       <c r="B12" t="s">
         <v>98</v>
       </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
       <c r="D12" t="s">
         <v>99</v>
       </c>
@@ -1773,6 +1783,9 @@
       <c r="A14" t="s">
         <v>5</v>
       </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
       <c r="D14" t="s">
         <v>99</v>
       </c>
@@ -1807,6 +1820,9 @@
       <c r="B16" t="s">
         <v>98</v>
       </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
       <c r="D16" t="s">
         <v>99</v>
       </c>
@@ -1826,6 +1842,9 @@
       </c>
       <c r="B17" t="s">
         <v>98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
       </c>
       <c r="D17" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
update docs for next release.
</commit_message>
<xml_diff>
--- a/docs/WorkingStatus.xlsx
+++ b/docs/WorkingStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kitoh\source\aliceconv\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D87967-9BAE-48C0-8A00-E041049E2433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DB08A8-8472-4602-8250-12B5DF605C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{FF061521-1F21-4413-9E31-090A18910087}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="102">
   <si>
     <t>リトルプリンセス</t>
   </si>
@@ -420,6 +420,10 @@
   </si>
   <si>
     <t>〇 (PC88MML)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〇 (MCL)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1624,7 +1628,7 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1737,13 +1741,16 @@
       <c r="C10" t="s">
         <v>100</v>
       </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">

</xml_diff>